<commit_message>
added 3 user stories
</commit_message>
<xml_diff>
--- a/User_Stories.xlsx
+++ b/User_Stories.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\styli\OneDrive\Υπολογιστής\projectpithia\Pithia\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7034FDC7-422B-4E1D-A2EA-514871FFCB22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Διεργασία" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Product backlog Pithia" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Acceptance" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Διεργασία" sheetId="1" r:id="rId1"/>
+    <sheet name="Product backlog Pithia" sheetId="2" r:id="rId2"/>
+    <sheet name="Acceptance" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -22,24 +32,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="154">
   <si>
     <t xml:space="preserve"> Βήματα διεργασίας SCRUM</t>
   </si>
   <si>
-    <t xml:space="preserve">Δραστηριότητα/Εργασίες</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Αρμόδιος</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Δημιουργία Product backlog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Εισαγωγή User stories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product owner</t>
+    <t>Δραστηριότητα/Εργασίες</t>
+  </si>
+  <si>
+    <t>Αρμόδιος</t>
+  </si>
+  <si>
+    <t>Δημιουργία Product backlog</t>
+  </si>
+  <si>
+    <t>Εισαγωγή User stories</t>
+  </si>
+  <si>
+    <t>Product owner</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -48,103 +58,103 @@
     <t xml:space="preserve">Προτεραιοποίηση </t>
   </si>
   <si>
-    <t xml:space="preserve">Φάση Sprint (max 22 ημέρες διάρκεια - 1000 ανθρωποώρες)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint Planning (1η ημέρα)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ορισμός στόχου Sprint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product owner, Ομάδα SCRUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Επιλογή PBI's &amp; Εκτίμηση προσπάθειας</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ομάδα SCRUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Δημιουργία Sprint backlog (+ Tasks)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Αυτοοργάνωση ομάδας</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Εκτέλεση Sprint backlog (διάρκεια 2-4 εβδομάδες)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Αφαίρεση εμποδίων</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCRUM Master</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ημερήσιο SCRUM meeting (15' διάρκεια)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCRUM Master, Ομάδα SCRUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ανάπτυξη λειτουργιών των user stories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ενημέρωση Burn down διαγράμματος</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Επίξειξη και Αναδρομή Sprint</t>
+    <t>Φάση Sprint (max 22 ημέρες διάρκεια - 1000 ανθρωποώρες)</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Sprint Planning (1η ημέρα)</t>
+  </si>
+  <si>
+    <t>Ορισμός στόχου Sprint</t>
+  </si>
+  <si>
+    <t>Product owner, Ομάδα SCRUM</t>
+  </si>
+  <si>
+    <t>Επιλογή PBI's &amp; Εκτίμηση προσπάθειας</t>
+  </si>
+  <si>
+    <t>Ομάδα SCRUM</t>
+  </si>
+  <si>
+    <t>Δημιουργία Sprint backlog (+ Tasks)</t>
+  </si>
+  <si>
+    <t>Αυτοοργάνωση ομάδας</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>Εκτέλεση Sprint backlog (διάρκεια 2-4 εβδομάδες)</t>
+  </si>
+  <si>
+    <t>Αφαίρεση εμποδίων</t>
+  </si>
+  <si>
+    <t>SCRUM Master</t>
+  </si>
+  <si>
+    <t>Ημερήσιο SCRUM meeting (15' διάρκεια)</t>
+  </si>
+  <si>
+    <t>SCRUM Master, Ομάδα SCRUM</t>
+  </si>
+  <si>
+    <t>Ανάπτυξη λειτουργιών των user stories</t>
+  </si>
+  <si>
+    <t>Ενημέρωση Burn down διαγράμματος</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>Επίξειξη και Αναδρομή Sprint</t>
   </si>
   <si>
     <t xml:space="preserve">Sprint review (4 ώρες) </t>
   </si>
   <si>
-    <t xml:space="preserve">Ολοι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint retrospective (15' έκαστος)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ΕΦΑΡΜΟΓΗ Pithia(Pithia Project)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
+    <t>Ολοι</t>
+  </si>
+  <si>
+    <t>Sprint retrospective (15' έκαστος)</t>
+  </si>
+  <si>
+    <t>ΕΦΑΡΜΟΓΗ Pithia(Pithia Project)</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
   <si>
     <t xml:space="preserve">STORY </t>
   </si>
   <si>
-    <t xml:space="preserve">Περιγραφή</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Product owner)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Scrum Team)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(PO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ως &lt;τύπος χρήστη&gt;, θέλω να &lt;κάνω … &gt; ώστε να &lt;επωφεληθώ ...&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US01</t>
+    <t>Περιγραφή</t>
+  </si>
+  <si>
+    <t>Estimation</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>(Product owner)</t>
+  </si>
+  <si>
+    <t>(Scrum Team)</t>
+  </si>
+  <si>
+    <t>(PO)</t>
+  </si>
+  <si>
+    <t>Ως &lt;τύπος χρήστη&gt;, θέλω να &lt;κάνω … &gt; ώστε να &lt;επωφεληθώ ...&gt;</t>
+  </si>
+  <si>
+    <t>US01</t>
   </si>
   <si>
     <r>
@@ -159,21 +169,21 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="161"/>
       </rPr>
-      <t xml:space="preserve">login</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Στο UI εισάγω τα διαπιστευτήριά μου (αριθμος μητρωου, κωδικος) με τα οποία, μετά τον έλεγχο, εισάγομαι στην εφαρμογή.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US02</t>
+      <t>login</t>
+    </r>
+  </si>
+  <si>
+    <t>Στο UI εισάγω τα διαπιστευτήριά μου (αριθμος μητρωου, κωδικος) με τα οποία, μετά τον έλεγχο, εισάγομαι στην εφαρμογή.</t>
+  </si>
+  <si>
+    <t>US02</t>
   </si>
   <si>
     <r>
@@ -188,21 +198,21 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">logout</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Πατώντας "Logout",εξέρχομαι από την εφαρμογή.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US03</t>
+      <t>logout</t>
+    </r>
+  </si>
+  <si>
+    <t>Πατώντας "Logout",εξέρχομαι από την εφαρμογή.</t>
+  </si>
+  <si>
+    <t>US03</t>
   </si>
   <si>
     <r>
@@ -216,13 +226,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Bαθμολογία</t>
+      <t>Bαθμολογία</t>
     </r>
     <r>
       <rPr>
@@ -238,54 +248,54 @@
     <t xml:space="preserve">Πατώντας  την επιλογή ¨Βαθμολογία” από το μενού,θα μπορεί ο φοιτητης/τρια χρήστης να βλέπει τις βαθμολογίες του. </t>
   </si>
   <si>
-    <t xml:space="preserve">US04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ως  φοιτητής, θέλω να βλέπω  τη Δηλωσή μου.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Πατώντας την επιλογή “ Δήλωση” από το μενού,θα μπορεί ο ταυτοποιήμενος χρήστης να δει τα μαθήματα που έχει δηλώσει.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ως καθηγητής,θέλω να έχω δυνατότητα να Εισάγω  Βαθμολογία στους μαθητές που παρακολουθούν το μάθημα/μαθήματα που διδάσκω.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Δηλωση Βαθμολογιας" το οποιο θα οδηγει τον καθηγητη στη φορμα δηλωσης βαθμολογιας φοιτητων.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ως διαχειριστης,θελω να εχω δυνατοτητα να δημιουργω χ αριθμο κωδικων για χ φοιττηες.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Φοιτητες” η οποια θα τον οδηγει στο περιβαλλον διαχειρησης φοιτητων.Εκει,εκτος αλλων,θα υπαρχει κουμπι “Δημιουργια Κωδικων Φοιτητων” με το οποιο θα μπορει να δημιουργει παραμετρικο αριθμο φοιτητων</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ως καθηγητης που διδασκω καποιο μαθημα,θελω να εχω δυνατοτητα να οριζω τον αλγοριθμο βαση του οποιου θα υπολογιζεται ο τελικος βαθμος των φοιτητων στο μαθημα.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Τα μαθηματα μου” οπου,διαλεγωντας το μαθημα,θα του ανοιγει φορμα οπου,εκτος αλλων,θα μπορει να δηλωνει ποσοστα συμμετοχης διαφορων βαθμων του μαθηματος στον τελικο βαθμο(πχ,εργαστηριο,θεωρια και εργασιας)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User story</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ως logout χρηστης θέλω να κάνω login για να εχω προσβαση στο συστημα.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Κριτήρια αποδοχής</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
+    <t>US04</t>
+  </si>
+  <si>
+    <t>Ως  φοιτητής, θέλω να βλέπω  τη Δηλωσή μου.</t>
+  </si>
+  <si>
+    <t>Πατώντας την επιλογή “ Δήλωση” από το μενού,θα μπορεί ο ταυτοποιήμενος χρήστης να δει τα μαθήματα που έχει δηλώσει.</t>
+  </si>
+  <si>
+    <t>US05</t>
+  </si>
+  <si>
+    <t>Ως καθηγητής,θέλω να έχω δυνατότητα να Εισάγω  Βαθμολογία στους μαθητές που παρακολουθούν το μάθημα/μαθήματα που διδάσκω.</t>
+  </si>
+  <si>
+    <t>Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Δηλωση Βαθμολογιας" το οποιο θα οδηγει τον καθηγητη στη φορμα δηλωσης βαθμολογιας φοιτητων.</t>
+  </si>
+  <si>
+    <t>U06</t>
+  </si>
+  <si>
+    <t>Ως διαχειριστης,θελω να εχω δυνατοτητα να δημιουργω χ αριθμο κωδικων για χ φοιττηες.</t>
+  </si>
+  <si>
+    <t>Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Φοιτητες” η οποια θα τον οδηγει στο περιβαλλον διαχειρησης φοιτητων.Εκει,εκτος αλλων,θα υπαρχει κουμπι “Δημιουργια Κωδικων Φοιτητων” με το οποιο θα μπορει να δημιουργει παραμετρικο αριθμο φοιτητων</t>
+  </si>
+  <si>
+    <t>US07</t>
+  </si>
+  <si>
+    <t>Ως καθηγητης που διδασκω καποιο μαθημα,θελω να εχω δυνατοτητα να οριζω τον αλγοριθμο βαση του οποιου θα υπολογιζεται ο τελικος βαθμος των φοιτητων στο μαθημα.</t>
+  </si>
+  <si>
+    <t>Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Τα μαθηματα μου” οπου,διαλεγωντας το μαθημα,θα του ανοιγει φορμα οπου,εκτος αλλων,θα μπορει να δηλωνει ποσοστα συμμετοχης διαφορων βαθμων του μαθηματος στον τελικο βαθμο(πχ,εργαστηριο,θεωρια και εργασιας)</t>
+  </si>
+  <si>
+    <t>User story</t>
+  </si>
+  <si>
+    <t>Ως logout χρηστης θέλω να κάνω login για να εχω προσβαση στο συστημα.</t>
+  </si>
+  <si>
+    <t>Κριτήρια αποδοχής</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="16"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
@@ -302,14 +312,14 @@
         <family val="2"/>
         <charset val="161"/>
       </rPr>
-      <t xml:space="preserve">Logoout χρηστης μπαινει στο συστημα.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>Logoout χρηστης μπαινει στο συστημα.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -326,14 +336,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">οτι ειμαι logout και ειμαι στην φορμα εισαγωγης,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>οτι ειμαι logout και ειμαι στην φορμα εισαγωγης,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -350,14 +360,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">βαζω το ονομα χρηστη και τον κωδικο μου</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>βαζω το ονομα χρηστη και τον κωδικο μου</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -374,14 +384,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">παταω το κουμπι Συνδεση,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>παταω το κουμπι Συνδεση,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -398,7 +408,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα μου επιτρεπει προσβαση</t>
+      <t>το συστημα μου επιτρεπει προσβαση</t>
     </r>
     <r>
       <rPr>
@@ -418,16 +428,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">και μου εμφανιζει το παραθυρο εφαρμογης με το μενου επιλογων.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Ως ταυτοποιημένος χρήστης θέλω να κάνω logout.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t>και μου εμφανιζει το παραθυρο εφαρμογης με το μενου επιλογων.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ως ταυτοποιημένος χρήστης θέλω να κάνω logout.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="16"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
@@ -444,14 +454,14 @@
         <family val="2"/>
         <charset val="161"/>
       </rPr>
-      <t xml:space="preserve">Συνδεδεμενος χρηστης βγαινει απο το συστημα.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>Συνδεδεμενος χρηστης βγαινει απο το συστημα.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -468,14 +478,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">οτι ειμαι συνδεδεμενος στο συστημα,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>οτι ειμαι συνδεδεμενος στο συστημα,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -492,14 +502,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">παταων στο μενου το κουμπι Logout</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>παταων στο μενου το κουμπι Logout</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -516,14 +526,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">παταω “Ναι” οταν το συστημα με ρωταει αν θελω να βγω,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>παταω “Ναι” οταν το συστημα με ρωταει αν θελω να βγω,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -540,7 +550,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα με αποσυνδεει και με πηγαινει στη φορμα εισαγωγης.</t>
+      <t>το συστημα με αποσυνδεει και με πηγαινει στη φορμα εισαγωγης.</t>
     </r>
   </si>
   <si>
@@ -556,14 +566,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="161"/>
       </rPr>
-      <t xml:space="preserve">Bαθμολογία</t>
+      <t>Bαθμολογία</t>
     </r>
     <r>
       <rPr>
@@ -579,7 +589,7 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="16"/>
         <color rgb="FFC9211E"/>
         <rFont val="Calibri"/>
@@ -596,11 +606,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ο Φοιτητής</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t>Ο Φοιτητής</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="16"/>
         <color rgb="FFC9211E"/>
         <rFont val="Calibri"/>
@@ -623,14 +633,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Δεδομένου</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Δεδομένου</t>
     </r>
     <r>
       <rPr>
@@ -646,14 +656,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Όταν</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Όταν</t>
     </r>
     <r>
       <rPr>
@@ -669,14 +679,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Τότε</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Τότε</t>
     </r>
     <r>
       <rPr>
@@ -702,14 +712,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="161"/>
       </rPr>
-      <t xml:space="preserve">Δηλωσή</t>
+      <t>Δηλωσή</t>
     </r>
     <r>
       <rPr>
@@ -725,7 +735,7 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="16"/>
         <color rgb="FFC9211E"/>
         <rFont val="Calibri"/>
@@ -742,11 +752,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ο Φοιτητής  βλέπει τα μαθήματα που έχει δηλώσει στο</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t>Ο Φοιτητής  βλέπει τα μαθήματα που έχει δηλώσει στο</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="16"/>
         <color rgb="FFC9211E"/>
         <rFont val="Calibri"/>
@@ -763,13 +773,13 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">τρέχον εξάμηνο και σε παλαιότερα</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t>τρέχον εξάμηνο και σε παλαιότερα</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -786,11 +796,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">ότι είμαι φοιτητής</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t>ότι είμαι φοιτητής</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -803,14 +813,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Όταν</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Όταν</t>
     </r>
     <r>
       <rPr>
@@ -826,14 +836,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Τότε</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Τότε</t>
     </r>
     <r>
       <rPr>
@@ -859,14 +869,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="161"/>
       </rPr>
-      <t xml:space="preserve">Εισάγω  Βαθμολογία</t>
+      <t>Εισάγω  Βαθμολογία</t>
     </r>
     <r>
       <rPr>
@@ -882,7 +892,7 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="16"/>
         <color rgb="FFC9211E"/>
         <rFont val="Calibri"/>
@@ -899,23 +909,23 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ο καθηγητής  εισάγει τη βαθμολογία των μαθήματων</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">στους φοιτητές</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Δεδομένου</t>
+      <t>Ο καθηγητής  εισάγει τη βαθμολογία των μαθήματων</t>
+    </r>
+  </si>
+  <si>
+    <t>στους φοιτητές</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Δεδομένου</t>
     </r>
     <r>
       <rPr>
@@ -931,14 +941,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Οταν</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Οταν</t>
     </r>
     <r>
       <rPr>
@@ -954,7 +964,7 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -971,13 +981,13 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το σύστημα μου εμφανιζει ενα μενού από το οποίο επιλέγω το [ΜΑΘΗΜΑ] και το τύπο του μαθήματος[ΘΕΩΡΙΑ][ΕΡΓΑΣΤΗΡΙΟ]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t>το σύστημα μου εμφανιζει ενα μενού από το οποίο επιλέγω το [ΜΑΘΗΜΑ] και το τύπο του μαθήματος[ΘΕΩΡΙΑ][ΕΡΓΑΣΤΗΡΙΟ]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -1000,14 +1010,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Τότε</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Τότε</t>
     </r>
     <r>
       <rPr>
@@ -1023,14 +1033,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Και</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Και</t>
     </r>
     <r>
       <rPr>
@@ -1046,14 +1056,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Τότε</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Τότε</t>
     </r>
     <r>
       <rPr>
@@ -1069,14 +1079,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Οταν</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Οταν</t>
     </r>
     <r>
       <rPr>
@@ -1092,14 +1102,14 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Τότε</t>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Τότε</t>
     </r>
     <r>
       <rPr>
@@ -1113,12 +1123,12 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">US06</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
+    <t>US06</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="16"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
@@ -1135,14 +1145,14 @@
         <family val="2"/>
         <charset val="161"/>
       </rPr>
-      <t xml:space="preserve">Ο διαχειριστης παραγει εναν αριθμο κωδικων.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>Ο διαχειριστης παραγει εναν αριθμο κωδικων.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -1159,14 +1169,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">οτι ειμαι συνδεδεμενος ως διαχειριστης,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>οτι ειμαι συνδεδεμενος ως διαχειριστης,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -1183,14 +1193,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">παταων στο μενου το κουμπι Φοιτητες,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>παταων στο μενου το κουμπι Φοιτητες,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1207,14 +1217,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα με καθοδηγει στο περιβαλλον επεξεργασιας φοιτητων οπου υπαρχει φορμα παραγωγης κωδικων φοιτητων με πεδια ετος,αριθμος κωδικων φοιτητων,prefix και το κουμπι Παραγωγη</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>το συστημα με καθοδηγει στο περιβαλλον επεξεργασιας φοιτητων οπου υπαρχει φορμα παραγωγης κωδικων φοιτητων με πεδια ετος,αριθμος κωδικων φοιτητων,prefix και το κουμπι Παραγωγη</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -1237,8 +1247,8 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <i val="true"/>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1255,14 +1265,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">πατησω το κουμπι Παραγωγη,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>πατησω το κουμπι Παραγωγη,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1279,7 +1289,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα εμφανιζει μηνυμα της μορφης [χ κωδικοι δημιουργηθηκαν][διαδρομη για το ονομα αρχειου]</t>
+      <t>το συστημα εμφανιζει μηνυμα της μορφης [χ κωδικοι δημιουργηθηκαν][διαδρομη για το ονομα αρχειου]</t>
     </r>
   </si>
   <si>
@@ -1288,7 +1298,7 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="16"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
@@ -1305,14 +1315,14 @@
         <family val="2"/>
         <charset val="161"/>
       </rPr>
-      <t xml:space="preserve">Ο καθηγητης οριζει τον αλγοριθμο υπολογισμου του τελικου βαθμου.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>Ο καθηγητης οριζει τον αλγοριθμο υπολογισμου του τελικου βαθμου.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1329,14 +1339,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">οτι ειμαι συνδεδεμενος στο συστημα ως καθηγητης,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>οτι ειμαι συνδεδεμενος στο συστημα ως καθηγητης,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1353,14 +1363,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">επιλεγω απο το μενου την επιλογη Τα μαθηματα μου</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>επιλεγω απο το μενου την επιλογη Τα μαθηματα μου</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1377,14 +1387,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα με καθοδηγει στο περιβαλλον επεξεργασιας των μαθηματων μου οπου υπαρχει μια λιστα με τα μαθηματα που διδασκω και μια φορμα με πεδια:[Input][Label Ποσοστο συμμετοχης Θεωριας][Λιστα με τιμες απο 0% - 100%],[input][Label Ποσοστο συμμετοχης εργαστηριου][Λιστα με τιμες απο 0% εως 100%] και [Κουμπι Αποθηκευση]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>το συστημα με καθοδηγει στο περιβαλλον επεξεργασιας των μαθηματων μου οπου υπαρχει μια λιστα με τα μαθηματα που διδασκω και μια φορμα με πεδια:[Input][Label Ποσοστο συμμετοχης Θεωριας][Λιστα με τιμες απο 0% - 100%],[input][Label Ποσοστο συμμετοχης εργαστηριου][Λιστα με τιμες απο 0% εως 100%] και [Κουμπι Αποθηκευση]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1401,14 +1411,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">διαλεξω καποιο μαθηματα απο τη λιστα</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>διαλεξω καποιο μαθηματα απο τη λιστα</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1431,8 +1441,8 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <i val="true"/>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1449,14 +1459,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">συμπληρωσω το input για το ποσοστο συμμετοχης εργαστηριου</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>συμπληρωσω το input για το ποσοστο συμμετοχης εργαστηριου</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1473,14 +1483,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">πατησω το κουμπι Αποθηκευση,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>πατησω το κουμπι Αποθηκευση,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1497,14 +1507,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα εμφανιζει μηνυμα της μορφης [Καινουριος Αλγοριθμος Υπολογισμου Τελικου Βαθμου][χ% * βαθμος θεωριας]+[y%*βαθμος εργαστηριου][Κουμπι Αποθηκευση][Κουμπι Ακυρωση]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>το συστημα εμφανιζει μηνυμα της μορφης [Καινουριος Αλγοριθμος Υπολογισμου Τελικου Βαθμου][χ% * βαθμος θεωριας]+[y%*βαθμος εργαστηριου][Κουμπι Αποθηκευση][Κουμπι Ακυρωση]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1521,14 +1531,14 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">πατησω το κουμπι Αποθηκευση,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
+      <t>πατησω το κουμπι Αποθηκευση,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1545,19 +1555,689 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα αποθηκευει τον καινουριο αλγοριθμο.</t>
+      <t>το συστημα αποθηκευει τον καινουριο αλγοριθμο.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ως χρηστης,θελω να εχω δυνατοτητα να αλλαζω τον κωδικο μου.</t>
+  </si>
+  <si>
+    <t>US08</t>
+  </si>
+  <si>
+    <t>Οταν ο χρηστης θα μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Ο λογαριασμος μου” η οποια θα τον οδηγει στην φορμα οπου θα μπορει,εκτος αλλων,να αλλαζει τον κωδικο του.</t>
+  </si>
+  <si>
+    <t>US09</t>
+  </si>
+  <si>
+    <t>US10</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t xml:space="preserve">Σενάριο: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φοιτητης αλλαζει τον κωδικο του.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Δεδομένου </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>οτι ειμαι συνδεδεμενος στο συστημα ως χρηστης,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Όταν </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>παταω στο μενου την επιλογη “Ο λογαριαμος μου”,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τότε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα με καθοδηγει στο περιβαλλον επεξεργασιας του λογαριαμου μου οπου υπαρχει φορμα με πεδια Νεος Κωδικος και Επαναληψη Κωδικου και το κουμπι Αποθηκευση Κωδικου.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Οταν </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>γεμισω τα πεδια Νεος Κωδικος και Επαναληψη Κωδικου με το νεο μου κωδικο</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει μηνυμα της μορφης [Ο κωδικος αλλαξε],με κανει logout και μου ζηταει να ξαναμπω με τον καινουριο κωδικο.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ως καθηγητης που διδασκω καποιο εργαστηριο,θελω να εχω δυνατοτητα να προσθετω φοιτητες στο εργαστηριο.</t>
+  </si>
+  <si>
+    <t>Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Τα εργαστηρια μου” οπου,διαλεγωντας το εργαστηριο,θα του ανοιγει φορμα οπου,εκτος αλλων,θα υπαρχει δυνατοτηα προσθηκης φοιτητη.</t>
+  </si>
+  <si>
+    <t>Ως καθηγητης που διδασκω καποιο εργαστηριο,θελω να εχω δυνατοτητα να προσθετω/αφαιρω απουσιες στους φοιτιτες που παρακολουθουν το εργαστηριο</t>
+  </si>
+  <si>
+    <t>Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Τα εργαστηρια μου” οπου,διαλεγωντας το εργαστηριο,θα του ανοιγει φορμα οπου,εκτος αλλων,θα υπαρχει λιστα φοιτητων και κουμπι “Αυξηση απουσιων” και κουμπι “Μειωση απουσιων” διπλα σε καθε φοιτητη.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t xml:space="preserve">Σενάριο: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Καθηγητης Εργαστηριου προσθετη φοιτητη.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Δεδομένου </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>οτι ειμαι συνδεδεμενος στο συστημα ως καθηγητης,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Όταν </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>παταω στο μενου την επιλογη “Τα Εργαστηρια Μου”,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τότε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα με καθοδηγει στο περιβαλλον επεξεργασιας των εργαστηριων που διδασκω οπου υπαρχει λιστα με τα εργαστηρια μου.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Οταν </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>επιλεξω ενα εργαστηριο απο την λιστα,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει παραθυρο με τα στοιχεια του εργαστηριου και μια φορμα με πεδια ΑΜ φοιτητη και κουμπι Προσθηκη Φοιτητη στο εργαστηριο.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Οταν </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>γεμισω το πεδιο ΑΜ και πατησω το κουμπι Προσθηκη Φοιτητη Στο Εργαστηριο,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει μηνυμα της μορφης [Στοιχεια Φοιτητη] [Κουμπι Προσθηκη] [Κουμπι Ακυρωση]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Οταν </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>πατησω το κουμπι Προσθηκη,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει μηνυμα της μορφης [Στοιχεια Φοιτητη] προστεθηκε επιτυχως.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως καθηγητης που διδασκω καποιο εργαστηριο,θελω να εχω δυνατοτητα να προσθετω/αφαιρω απουσιες στους φοιτιτες που παρακολουθουν το εργαστηριο </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t xml:space="preserve">Σενάριο: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Καθηγητης Εργαστηριου αυξανη τις απουσιες καποιου φοιτητη.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει παραθυρο με τα στοιχεια του εργαστηριου οπου υπαρχει μια λιστα με ολους του φοιτητες της μορφης [ΑΜ][Ονομα Φοιτητη][Συνολο Απουσιων][Κουμπι Αυξηση Απουσιων][Μειωση Απουσιων].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Οταν </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>πατησω το κουμπι Αυξηση Απουσιων σε εναν φοιτητη,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει μηνυμα της μορφης [ΑΜ][Ονομα Φοιτητη][Κουμπι Αυξηση Απουσιων][Ακυρωση]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Οταν </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>πατησω το κουμπι Αυξηση Απουσιων,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει μηνυμα της μορφης [ΑΜ][Ονομα Φοιτητη][Συνολο Απουσιων] Απουσιες Αυξηθηκαν κατα ενα.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t xml:space="preserve">Σενάριο: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Καθηγητης Εργαστηριου μειωνει τις απουσιες καποιου φοιτητη.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει παραθυρο με τα στοιχεια του εργαστηριου οπου υπαρχει μια λιστα με ολους του φοιτητες της μορφης [ΑΜ][Ονομα Φοιτητη][Συνολο Απουσιων][Κουμπι Αυξηση Απουσιων][Κουμπι Μειωση Απουσιων].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Οταν </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>πατησω το κουμπι Μειωση Απουσιων,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει μηνυμα της μορφης [ΑΜ][Ονομα Φοιτητη][Κουμπι Μειωση Απουσιων][Ακυρωση]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Τοτε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>το συστημα εμφανιζει μηνυμα της μορφης [ΑΜ][Ονομα Φοιτητη][Συνολο Απουσιων] Απουσιες Μειωθηκαν κατα ενα.</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="28">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1566,22 +2246,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1596,7 +2261,7 @@
       <charset val="161"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1604,7 +2269,7 @@
       <charset val="161"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1612,7 +2277,7 @@
       <charset val="161"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1627,7 +2292,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1642,7 +2307,7 @@
       <charset val="161"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -1650,7 +2315,7 @@
       <charset val="161"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
@@ -1665,7 +2330,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1673,7 +2338,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -1687,7 +2352,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1701,7 +2366,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1709,7 +2374,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
@@ -1717,7 +2382,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -1725,8 +2390,8 @@
       <charset val="161"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
+      <b/>
+      <i/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1734,8 +2399,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
+      <b/>
+      <i/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
@@ -1757,12 +2422,26 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <color rgb="FFC9211E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1798,7 +2477,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1806,185 +2485,121 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="41">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="36">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="16" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2043,35 +2658,343 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.57"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" s="3" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2081,37 +3004,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" s="7" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+    <row r="4" spans="1:9" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" s="10" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+    <row r="7" spans="1:9" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -2121,7 +3044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" s="7" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -2129,43 +3052,43 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" s="7" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2173,44 +3096,44 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="12"/>
-      <c r="E16" s="0" t="s">
+      <c r="E16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -2220,98 +3143,90 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="20.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="12.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="14" width="8.67"/>
+    <col min="1" max="1" width="7.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="52" style="14" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="14" customWidth="1"/>
+    <col min="6" max="1025" width="8.7109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="true" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" s="15" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>31</v>
       </c>
@@ -2328,7 +3243,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="17" t="s">
         <v>36</v>
@@ -2341,13 +3256,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="18"/>
     </row>
-    <row r="5" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>40</v>
       </c>
@@ -2358,7 +3273,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="72.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -2369,7 +3284,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="65.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>46</v>
       </c>
@@ -2380,7 +3295,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="89.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>49</v>
       </c>
@@ -2391,7 +3306,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="86.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" ht="86.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>52</v>
       </c>
@@ -2402,7 +3317,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="123.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" ht="123.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>55</v>
       </c>
@@ -2413,7 +3328,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="113.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>58</v>
       </c>
@@ -2424,120 +3339,135 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-    </row>
-    <row r="14" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-    </row>
-    <row r="15" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="36"/>
+    </row>
+    <row r="14" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="36"/>
+    </row>
+    <row r="15" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
     </row>
-    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
     </row>
-    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
     </row>
-    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
     </row>
-    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
     </row>
-    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
     </row>
-    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
     </row>
-    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
     </row>
-    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
     </row>
-    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
     </row>
-    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
     </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
     </row>
-    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
     </row>
-    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
     </row>
-    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
     </row>
-    <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
     </row>
-    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
     </row>
-    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A2:B69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:AMK113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="82.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="21" width="11.52"/>
+    <col min="1" max="1" width="11.5703125" style="21"/>
+    <col min="2" max="2" width="82.140625" style="21" customWidth="1"/>
+    <col min="3" max="1025" width="11.5703125" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>31</v>
       </c>
@@ -2545,7 +3475,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>40</v>
       </c>
@@ -2553,43 +3483,43 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="27" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="27"/>
     </row>
-    <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>43</v>
       </c>
@@ -2597,39 +3527,39 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="27" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:2" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="28" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>46</v>
       </c>
@@ -2637,32 +3567,32 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="B21" s="32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="33" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" s="33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="B24" s="33" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>49</v>
       </c>
@@ -2670,32 +3600,32 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="B28" s="32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" s="33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" s="33" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="B31" s="33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
         <v>52</v>
       </c>
@@ -2703,67 +3633,67 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" s="31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" s="32" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" s="33" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" s="33" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="B39" s="33" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="B40" s="33" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="B41" s="33" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="B43" s="33" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" s="33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" s="33" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="s">
         <v>97</v>
       </c>
@@ -2771,49 +3701,49 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" s="26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" s="27" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" s="27" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:2" ht="81" x14ac:dyDescent="0.25">
       <c r="A52" s="27"/>
       <c r="B52" s="28" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="27"/>
       <c r="B53" s="27" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" s="28" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:2" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B55" s="28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
         <v>58</v>
       </c>
@@ -2821,71 +3751,371 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B58" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:2" ht="42" x14ac:dyDescent="0.25">
       <c r="B59" s="26" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:2" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B60" s="28" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B61" s="28" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:2" ht="141.75" x14ac:dyDescent="0.25">
       <c r="B62" s="28" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B63" s="28" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:2" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B64" s="28" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B65" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" s="28" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:3" ht="81" x14ac:dyDescent="0.25">
       <c r="B67" s="28" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" s="28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" s="28" t="s">
         <v>116</v>
       </c>
     </row>
+    <row r="70" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+      <c r="A70" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B70" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="38"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="38"/>
+      <c r="B71" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" s="38"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="38"/>
+      <c r="B72" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72" s="38"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="38"/>
+      <c r="B73" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C73" s="38"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="38"/>
+      <c r="B74" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" s="38"/>
+    </row>
+    <row r="75" spans="1:3" ht="84" x14ac:dyDescent="0.25">
+      <c r="A75" s="28"/>
+      <c r="B75" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C75" s="38"/>
+    </row>
+    <row r="76" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="38"/>
+      <c r="B76" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" s="38"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="38"/>
+      <c r="B77" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C77" s="38"/>
+    </row>
+    <row r="78" spans="1:3" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="38"/>
+      <c r="B78" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" s="38"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="38"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="38"/>
+    </row>
+    <row r="80" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+      <c r="A80" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" s="35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="38"/>
+      <c r="B81" s="40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="38"/>
+      <c r="B82" s="26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+      <c r="A83" s="38"/>
+      <c r="B83" s="27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="38"/>
+      <c r="B84" s="27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A85" s="28"/>
+      <c r="B85" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="38"/>
+      <c r="B86" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="38"/>
+      <c r="B87" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="38"/>
+      <c r="B88" s="28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A89" s="38"/>
+      <c r="B89" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="38"/>
+      <c r="B90" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="38"/>
+      <c r="B91" s="28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A92" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="B92" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" s="38"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="38"/>
+      <c r="B93" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C93" s="38"/>
+    </row>
+    <row r="94" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+      <c r="A94" s="38"/>
+      <c r="B94" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C94" s="38"/>
+    </row>
+    <row r="95" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+      <c r="A95" s="38"/>
+      <c r="B95" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C95" s="38"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="38"/>
+      <c r="B96" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C96" s="38"/>
+    </row>
+    <row r="97" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A97" s="28"/>
+      <c r="B97" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="C97" s="38"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="38"/>
+      <c r="B98" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C98" s="38"/>
+    </row>
+    <row r="99" spans="1:3" ht="81" x14ac:dyDescent="0.25">
+      <c r="A99" s="38"/>
+      <c r="B99" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C99" s="38"/>
+    </row>
+    <row r="100" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="38"/>
+      <c r="B100" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C100" s="38"/>
+    </row>
+    <row r="101" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="38"/>
+      <c r="B101" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C101" s="38"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="38"/>
+      <c r="B102" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C102" s="38"/>
+    </row>
+    <row r="103" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="38"/>
+      <c r="B103" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C103" s="38"/>
+    </row>
+    <row r="104" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+      <c r="A104" s="38"/>
+      <c r="B104" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C104" s="38"/>
+    </row>
+    <row r="105" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+      <c r="A105" s="38"/>
+      <c r="B105" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C105" s="38"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="38"/>
+      <c r="B106" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C106" s="38"/>
+    </row>
+    <row r="107" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A107" s="38"/>
+      <c r="B107" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="C107" s="38"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="38"/>
+      <c r="B108" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C108" s="38"/>
+    </row>
+    <row r="109" spans="1:3" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="A109" s="38"/>
+      <c r="B109" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C109" s="38"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="38"/>
+      <c r="B110" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C110" s="38"/>
+    </row>
+    <row r="111" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="38"/>
+      <c r="B111" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C111" s="38"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="38"/>
+      <c r="B112" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C112" s="38"/>
+    </row>
+    <row r="113" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="38"/>
+      <c r="B113" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C113" s="38"/>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <phoneticPr fontId="25" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Changes: 1)Added domain model UML.
</commit_message>
<xml_diff>
--- a/User_Stories.xlsx
+++ b/User_Stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Διεργασία" sheetId="1" state="visible" r:id="rId2"/>
@@ -647,7 +647,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">  βλέπει τη βαθμολογία των μαθημάτων του</t>
+      <t xml:space="preserve">βλέπει τη βαθμολογία των μαθημάτων του</t>
     </r>
   </si>
   <si>
@@ -3077,7 +3077,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.41"/>
@@ -3310,7 +3310,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -3590,8 +3590,8 @@
   </sheetPr>
   <dimension ref="A2:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C106" activeCellId="0" sqref="C106"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B112" activeCellId="0" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3706,7 +3706,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="34" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Allages: 1)Ebala to eniaiologiko montelo mesa se ksexwristo fakelo.
</commit_message>
<xml_diff>
--- a/User_Stories.xlsx
+++ b/User_Stories.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="162">
   <si>
     <t xml:space="preserve"> Βήματα διεργασίας SCRUM</t>
   </si>
@@ -772,11 +772,27 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ο καθηγητής  εισάγει τη βαθμολογία των μαθήματων</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">στους φοιτητές</t>
+      <t xml:space="preserve">Ο καθηγητής  εισάγει τη βαθμολογία </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">στους φοιτητές του</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> μαθήματος</t>
+    </r>
   </si>
   <si>
     <r>
@@ -2548,7 +2564,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2741,6 +2757,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -2986,7 +3008,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3077,7 +3099,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.41"/>
@@ -3590,8 +3612,8 @@
   </sheetPr>
   <dimension ref="A2:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B112" activeCellId="0" sqref="B112"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3739,64 +3761,60 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="34" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="23" t="s">
-        <v>91</v>
-      </c>
-    </row>
+    <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40" s="37" t="s">
         <v>53</v>
@@ -3809,39 +3827,39 @@
     </row>
     <row r="42" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="81" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="29"/>
       <c r="B45" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="29"/>
       <c r="B46" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3849,7 +3867,7 @@
         <v>55</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3859,57 +3877,57 @@
     </row>
     <row r="52" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="81" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3931,49 +3949,49 @@
     <row r="65" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="39"/>
       <c r="B65" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C65" s="39"/>
     </row>
     <row r="66" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="39"/>
       <c r="B66" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C66" s="39"/>
     </row>
     <row r="67" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="39"/>
       <c r="B67" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C67" s="39"/>
     </row>
     <row r="68" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="30"/>
       <c r="B68" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C68" s="39"/>
     </row>
     <row r="69" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="39"/>
       <c r="B69" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C69" s="39"/>
     </row>
     <row r="70" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="39"/>
       <c r="B70" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C70" s="39"/>
     </row>
     <row r="71" customFormat="false" ht="60.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="39"/>
       <c r="B71" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C71" s="39"/>
     </row>
@@ -3999,61 +4017,61 @@
     <row r="75" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="39"/>
       <c r="B75" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="39"/>
       <c r="B76" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="39"/>
       <c r="B77" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="30"/>
       <c r="B78" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="39"/>
       <c r="B79" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="60.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="39"/>
       <c r="B80" s="30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="39"/>
       <c r="B81" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="39"/>
       <c r="B82" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="39"/>
       <c r="B83" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="39"/>
       <c r="B84" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4061,7 +4079,7 @@
         <v>64</v>
       </c>
       <c r="B85" s="37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C85" s="39"/>
     </row>
@@ -4075,140 +4093,140 @@
     <row r="87" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="39"/>
       <c r="B87" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C87" s="39"/>
     </row>
     <row r="88" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="39"/>
       <c r="B88" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C88" s="39"/>
     </row>
     <row r="89" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="39"/>
       <c r="B89" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C89" s="39"/>
     </row>
     <row r="90" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="30"/>
       <c r="B90" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C90" s="39"/>
     </row>
     <row r="91" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="39"/>
       <c r="B91" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C91" s="39"/>
     </row>
     <row r="92" customFormat="false" ht="81" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="39"/>
       <c r="B92" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C92" s="39"/>
     </row>
     <row r="93" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="39"/>
       <c r="B93" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C93" s="39"/>
     </row>
     <row r="94" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="39"/>
       <c r="B94" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C94" s="39"/>
     </row>
     <row r="95" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="39"/>
       <c r="B95" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C95" s="39"/>
     </row>
     <row r="96" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="39"/>
       <c r="B96" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C96" s="39"/>
     </row>
     <row r="97" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="39"/>
       <c r="B97" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C97" s="39"/>
     </row>
     <row r="98" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="39"/>
       <c r="B98" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C98" s="39"/>
     </row>
     <row r="99" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="39"/>
       <c r="B99" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C99" s="39"/>
     </row>
     <row r="100" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="39"/>
       <c r="B100" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C100" s="39"/>
     </row>
     <row r="101" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="39"/>
       <c r="B101" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C101" s="39"/>
     </row>
     <row r="102" customFormat="false" ht="101.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="39"/>
       <c r="B102" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C102" s="39"/>
     </row>
     <row r="103" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="39"/>
       <c r="B103" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C103" s="39"/>
     </row>
     <row r="104" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="39"/>
       <c r="B104" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C104" s="39"/>
     </row>
     <row r="105" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="39"/>
       <c r="B105" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C105" s="39"/>
     </row>
     <row r="106" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="39"/>
       <c r="B106" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C106" s="39"/>
     </row>
@@ -4217,7 +4235,7 @@
         <v>67</v>
       </c>
       <c r="B108" s="41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4229,91 +4247,91 @@
     <row r="110" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="39"/>
       <c r="B110" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="39"/>
       <c r="B111" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="39"/>
       <c r="B112" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="30"/>
       <c r="B113" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="39"/>
       <c r="B114" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="39"/>
       <c r="B115" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="39"/>
       <c r="B116" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="39"/>
       <c r="B117" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="39"/>
       <c r="B118" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="39"/>
       <c r="B119" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="39"/>
       <c r="B120" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="39"/>
       <c r="B121" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="39"/>
       <c r="B122" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="39"/>
       <c r="B123" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="39"/>
       <c r="B124" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Changes: updated domain model.
</commit_message>
<xml_diff>
--- a/User_Stories.xlsx
+++ b/User_Stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Διεργασία" sheetId="1" state="visible" r:id="rId2"/>
@@ -170,7 +170,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Στο UI εισάγω τα διαπιστευτήριά μου (αριθμος μητρωου, κωδικος) με τα οποία, μετά τον έλεγχο, εισάγομαι στην εφαρμογή.</t>
+    <t xml:space="preserve">Στο UI εισάγω τα διαπιστευτήριά μου (ονομα χρηστη, κωδικος) με τα οποία, μετά τον έλεγχο, εισάγομαι στην εφαρμογή.</t>
   </si>
   <si>
     <t xml:space="preserve">US02</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">US05</t>
   </si>
   <si>
-    <t xml:space="preserve">Ως καθηγητής,θέλω να έχω δυνατότητα να Εισάγω  Βαθμολογία στους μαθητές που παρακολουθούν το μάθημα/μαθήματα που διδάσκω.</t>
+    <t xml:space="preserve">Ως καθηγητής,θέλω να έχω δυνατότητα να Εισάγω  Βαθμολογία στους φοιτιτές/τριες που παρακολουθούν το μάθημα/μαθήματα που διδάσκω(είτε είναι θεωρία ειτέ είναι εργαστήρια).</t>
   </si>
   <si>
     <t xml:space="preserve">Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Δηλωση Βαθμολογιας" το οποιο θα οδηγει τον καθηγητη στη φορμα δηλωσης βαθμολογιας φοιτητων.</t>
@@ -772,26 +772,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ο καθηγητής  εισάγει τη βαθμολογία </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">στους φοιτητές του</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> μαθήματος</t>
+      <t xml:space="preserve">Ο καθηγητής  εισάγει τη βαθμολογία στους φοιτητές του μαθήματος</t>
     </r>
   </si>
   <si>
@@ -2564,7 +2545,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2757,12 +2738,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -3008,7 +2983,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3099,7 +3074,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.41"/>
@@ -3332,8 +3307,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3612,7 +3587,7 @@
   </sheetPr>
   <dimension ref="A2:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>

</xml_diff>